<commit_message>
Elisabettagori patch 1 (#54)
* Update results.json

* Generated results

---------

Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/RESULTS/results.xlsx
+++ b/RESULTS/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="558">
   <si>
     <t>Fornitore</t>
   </si>
@@ -559,6 +559,12 @@
     <t>2023-04-20</t>
   </si>
   <si>
+    <t>LAB,RAD,RSA</t>
+  </si>
+  <si>
+    <t>2023-11-10</t>
+  </si>
+  <si>
     <t>APEIRON</t>
   </si>
   <si>
@@ -598,7 +604,7 @@
     <t>2303.05.01.00</t>
   </si>
   <si>
-    <t>2308.06.00.00</t>
+    <t>2308.06.00.00, 2311.07.00.00</t>
   </si>
   <si>
     <t>P4PVACCINAZIONI</t>
@@ -1069,6 +1075,9 @@
     <t>5.10, 5.11, 5.13, 5.13.3, 5.14, 5.22</t>
   </si>
   <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
     <t>IE-DEGENTI</t>
   </si>
   <si>
@@ -1102,6 +1111,15 @@
     <t>SSI</t>
   </si>
   <si>
+    <t>HEALTH INSIDE</t>
+  </si>
+  <si>
+    <t>SADI HEALTH</t>
+  </si>
+  <si>
+    <t>V.1.0</t>
+  </si>
+  <si>
     <t>Hi.Tech</t>
   </si>
   <si>
@@ -1322,9 +1340,6 @@
   </si>
   <si>
     <t>ASAP</t>
-  </si>
-  <si>
-    <t>V.1.0</t>
   </si>
   <si>
     <t>RIS</t>
@@ -2004,7 +2019,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H207"/>
+  <dimension ref="A1:H211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3183,22 +3198,22 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" t="s">
+        <v>179</v>
+      </c>
+      <c r="E51" t="s">
         <v>181</v>
       </c>
-      <c r="C51" t="s">
-        <v>164</v>
-      </c>
-      <c r="E51" t="s">
-        <v>73</v>
-      </c>
       <c r="F51" t="s">
         <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
       <c r="H51" t="s">
         <v>14</v>
@@ -3206,22 +3221,22 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="H52" t="s">
         <v>14</v>
@@ -3229,13 +3244,13 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C53" t="s">
-        <v>184</v>
+        <v>111</v>
       </c>
       <c r="E53" t="s">
         <v>11</v>
@@ -3244,7 +3259,7 @@
         <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="H53" t="s">
         <v>14</v>
@@ -3252,7 +3267,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
         <v>185</v>
@@ -3260,17 +3275,14 @@
       <c r="C54" t="s">
         <v>186</v>
       </c>
-      <c r="D54" t="s">
-        <v>187</v>
-      </c>
       <c r="E54" t="s">
-        <v>188</v>
+        <v>11</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="H54" t="s">
         <v>14</v>
@@ -3281,13 +3293,16 @@
         <v>159</v>
       </c>
       <c r="B55" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" t="s">
         <v>189</v>
       </c>
-      <c r="C55" t="s">
-        <v>164</v>
-      </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -3304,19 +3319,19 @@
         <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="E56" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
         <v>12</v>
       </c>
       <c r="G56" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="H56" t="s">
         <v>14</v>
@@ -3324,7 +3339,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B57" t="s">
         <v>192</v>
@@ -3332,17 +3347,14 @@
       <c r="C57" t="s">
         <v>193</v>
       </c>
-      <c r="D57" t="s">
-        <v>194</v>
-      </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s">
         <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="H57" t="s">
         <v>14</v>
@@ -3353,10 +3365,13 @@
         <v>166</v>
       </c>
       <c r="B58" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" t="s">
         <v>195</v>
       </c>
-      <c r="C58" t="s">
-        <v>184</v>
+      <c r="D58" t="s">
+        <v>196</v>
       </c>
       <c r="E58" t="s">
         <v>86</v>
@@ -3365,7 +3380,7 @@
         <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>196</v>
+        <v>105</v>
       </c>
       <c r="H58" t="s">
         <v>14</v>
@@ -3373,22 +3388,22 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
         <v>197</v>
       </c>
       <c r="C59" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
         <v>198</v>
-      </c>
-      <c r="E59" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" t="s">
-        <v>196</v>
       </c>
       <c r="H59" t="s">
         <v>14</v>
@@ -3402,16 +3417,16 @@
         <v>199</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="F60" t="s">
         <v>12</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="H60" t="s">
         <v>14</v>
@@ -3419,16 +3434,13 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
-      </c>
-      <c r="D61" t="s">
-        <v>202</v>
+        <v>58</v>
       </c>
       <c r="E61" t="s">
         <v>11</v>
@@ -3437,7 +3449,7 @@
         <v>12</v>
       </c>
       <c r="G61" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H61" t="s">
         <v>14</v>
@@ -3445,22 +3457,25 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>202</v>
       </c>
       <c r="C62" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" t="s">
         <v>204</v>
       </c>
       <c r="E62" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F62" t="s">
         <v>12</v>
       </c>
       <c r="G62" t="s">
-        <v>63</v>
+        <v>205</v>
       </c>
       <c r="H62" t="s">
         <v>14</v>
@@ -3468,22 +3483,22 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="C63" t="s">
         <v>206</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F63" t="s">
         <v>12</v>
       </c>
       <c r="G63" t="s">
-        <v>207</v>
+        <v>63</v>
       </c>
       <c r="H63" t="s">
         <v>14</v>
@@ -3491,22 +3506,22 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B64" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" t="s">
         <v>208</v>
       </c>
-      <c r="C64" t="s">
+      <c r="E64" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
         <v>209</v>
-      </c>
-      <c r="E64" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" t="s">
-        <v>124</v>
       </c>
       <c r="H64" t="s">
         <v>14</v>
@@ -3514,22 +3529,22 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C65" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="E65" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="H65" t="s">
         <v>14</v>
@@ -3537,22 +3552,22 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C66" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E66" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="F66" t="s">
         <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="H66" t="s">
         <v>14</v>
@@ -3560,22 +3575,22 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" t="s">
         <v>214</v>
       </c>
-      <c r="B67" t="s">
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
         <v>215</v>
-      </c>
-      <c r="C67" t="s">
-        <v>14</v>
-      </c>
-      <c r="E67" t="s">
-        <v>216</v>
-      </c>
-      <c r="F67" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" t="s">
-        <v>217</v>
       </c>
       <c r="H67" t="s">
         <v>14</v>
@@ -3583,22 +3598,22 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
+        <v>216</v>
+      </c>
+      <c r="B68" t="s">
+        <v>217</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
         <v>218</v>
       </c>
-      <c r="B68" t="s">
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
         <v>219</v>
-      </c>
-      <c r="C68" t="s">
-        <v>58</v>
-      </c>
-      <c r="E68" t="s">
-        <v>86</v>
-      </c>
-      <c r="F68" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" t="s">
-        <v>220</v>
       </c>
       <c r="H68" t="s">
         <v>14</v>
@@ -3606,22 +3621,22 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
+        <v>220</v>
+      </c>
+      <c r="B69" t="s">
         <v>221</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s">
         <v>222</v>
-      </c>
-      <c r="C69" t="s">
-        <v>223</v>
-      </c>
-      <c r="E69" t="s">
-        <v>108</v>
-      </c>
-      <c r="F69" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" t="s">
-        <v>55</v>
       </c>
       <c r="H69" t="s">
         <v>14</v>
@@ -3629,22 +3644,22 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
+        <v>223</v>
+      </c>
+      <c r="B70" t="s">
         <v>224</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>225</v>
       </c>
-      <c r="C70" t="s">
-        <v>226</v>
-      </c>
       <c r="E70" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="F70" t="s">
         <v>12</v>
       </c>
       <c r="G70" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="H70" t="s">
         <v>14</v>
@@ -3652,22 +3667,22 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
+        <v>226</v>
+      </c>
+      <c r="B71" t="s">
         <v>227</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>228</v>
       </c>
-      <c r="C71" t="s">
-        <v>58</v>
-      </c>
       <c r="E71" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="H71" t="s">
         <v>14</v>
@@ -3678,19 +3693,19 @@
         <v>229</v>
       </c>
       <c r="B72" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C72" t="s">
-        <v>230</v>
+        <v>58</v>
       </c>
       <c r="E72" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F72" t="s">
         <v>12</v>
       </c>
       <c r="G72" t="s">
-        <v>231</v>
+        <v>102</v>
       </c>
       <c r="H72" t="s">
         <v>14</v>
@@ -3698,22 +3713,22 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
+        <v>231</v>
+      </c>
+      <c r="B73" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" t="s">
         <v>232</v>
       </c>
-      <c r="B73" t="s">
+      <c r="E73" t="s">
+        <v>86</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
         <v>233</v>
-      </c>
-      <c r="C73" t="s">
-        <v>234</v>
-      </c>
-      <c r="E73" t="s">
-        <v>27</v>
-      </c>
-      <c r="F73" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" t="s">
-        <v>235</v>
       </c>
       <c r="H73" t="s">
         <v>14</v>
@@ -3721,22 +3736,22 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B74" t="s">
+        <v>235</v>
+      </c>
+      <c r="C74" t="s">
         <v>236</v>
       </c>
-      <c r="C74" t="s">
-        <v>234</v>
-      </c>
       <c r="E74" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F74" t="s">
         <v>12</v>
       </c>
       <c r="G74" t="s">
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="H74" t="s">
         <v>14</v>
@@ -3744,22 +3759,22 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B75" t="s">
         <v>238</v>
       </c>
       <c r="C75" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E75" t="s">
-        <v>240</v>
+        <v>108</v>
       </c>
       <c r="F75" t="s">
         <v>12</v>
       </c>
       <c r="G75" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="H75" t="s">
         <v>14</v>
@@ -3767,22 +3782,22 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" t="s">
+        <v>240</v>
+      </c>
+      <c r="C76" t="s">
         <v>241</v>
       </c>
-      <c r="B76" t="s">
+      <c r="E76" t="s">
         <v>242</v>
       </c>
-      <c r="C76" t="s">
-        <v>243</v>
-      </c>
-      <c r="E76" t="s">
-        <v>18</v>
-      </c>
       <c r="F76" t="s">
         <v>12</v>
       </c>
       <c r="G76" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="H76" t="s">
         <v>14</v>
@@ -3790,13 +3805,13 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B77" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" t="s">
         <v>245</v>
-      </c>
-      <c r="C77" t="s">
-        <v>243</v>
       </c>
       <c r="E77" t="s">
         <v>18</v>
@@ -3805,7 +3820,7 @@
         <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H77" t="s">
         <v>14</v>
@@ -3813,22 +3828,22 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B78" t="s">
+        <v>247</v>
+      </c>
+      <c r="C78" t="s">
+        <v>245</v>
+      </c>
+      <c r="E78" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" t="s">
         <v>246</v>
-      </c>
-      <c r="C78" t="s">
-        <v>247</v>
-      </c>
-      <c r="E78" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" t="s">
-        <v>235</v>
       </c>
       <c r="H78" t="s">
         <v>14</v>
@@ -3836,22 +3851,22 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B79" t="s">
         <v>248</v>
       </c>
       <c r="C79" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E79" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="F79" t="s">
         <v>12</v>
       </c>
       <c r="G79" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="H79" t="s">
         <v>14</v>
@@ -3859,22 +3874,22 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B80" t="s">
         <v>250</v>
       </c>
       <c r="C80" t="s">
+        <v>249</v>
+      </c>
+      <c r="E80" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s">
         <v>251</v>
-      </c>
-      <c r="E80" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" t="s">
-        <v>252</v>
       </c>
       <c r="H80" t="s">
         <v>14</v>
@@ -3882,22 +3897,22 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B81" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" t="s">
         <v>253</v>
       </c>
-      <c r="C81" t="s">
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
         <v>254</v>
-      </c>
-      <c r="E81" t="s">
-        <v>73</v>
-      </c>
-      <c r="F81" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" t="s">
-        <v>78</v>
       </c>
       <c r="H81" t="s">
         <v>14</v>
@@ -3905,22 +3920,22 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
+        <v>243</v>
+      </c>
+      <c r="B82" t="s">
         <v>255</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>256</v>
       </c>
-      <c r="C82" t="s">
-        <v>257</v>
-      </c>
       <c r="E82" t="s">
-        <v>258</v>
+        <v>73</v>
       </c>
       <c r="F82" t="s">
         <v>12</v>
       </c>
       <c r="G82" t="s">
-        <v>259</v>
+        <v>78</v>
       </c>
       <c r="H82" t="s">
         <v>14</v>
@@ -3928,22 +3943,22 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B83" t="s">
+        <v>258</v>
+      </c>
+      <c r="C83" t="s">
+        <v>259</v>
+      </c>
+      <c r="E83" t="s">
         <v>260</v>
       </c>
-      <c r="C83" t="s">
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
         <v>261</v>
-      </c>
-      <c r="E83" t="s">
-        <v>258</v>
-      </c>
-      <c r="F83" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" t="s">
-        <v>259</v>
       </c>
       <c r="H83" t="s">
         <v>14</v>
@@ -3951,22 +3966,22 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
+        <v>257</v>
+      </c>
+      <c r="B84" t="s">
         <v>262</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>263</v>
       </c>
-      <c r="C84" t="s">
-        <v>264</v>
-      </c>
       <c r="E84" t="s">
-        <v>27</v>
+        <v>260</v>
       </c>
       <c r="F84" t="s">
         <v>12</v>
       </c>
       <c r="G84" t="s">
-        <v>105</v>
+        <v>261</v>
       </c>
       <c r="H84" t="s">
         <v>14</v>
@@ -3974,22 +3989,22 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B85" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C85" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E85" t="s">
-        <v>240</v>
+        <v>27</v>
       </c>
       <c r="F85" t="s">
         <v>12</v>
       </c>
       <c r="G85" t="s">
-        <v>207</v>
+        <v>105</v>
       </c>
       <c r="H85" t="s">
         <v>14</v>
@@ -3997,22 +4012,22 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
+        <v>264</v>
+      </c>
+      <c r="B86" t="s">
         <v>265</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>266</v>
       </c>
-      <c r="C86" t="s">
-        <v>239</v>
-      </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>242</v>
       </c>
       <c r="F86" t="s">
         <v>12</v>
       </c>
       <c r="G86" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="H86" t="s">
         <v>14</v>
@@ -4026,16 +4041,16 @@
         <v>268</v>
       </c>
       <c r="C87" t="s">
-        <v>14</v>
+        <v>241</v>
       </c>
       <c r="E87" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="F87" t="s">
         <v>12</v>
       </c>
       <c r="G87" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="H87" t="s">
         <v>14</v>
@@ -4049,16 +4064,16 @@
         <v>270</v>
       </c>
       <c r="C88" t="s">
-        <v>271</v>
+        <v>14</v>
       </c>
       <c r="E88" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>272</v>
+        <v>55</v>
       </c>
       <c r="H88" t="s">
         <v>14</v>
@@ -4066,22 +4081,22 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
+        <v>271</v>
+      </c>
+      <c r="B89" t="s">
+        <v>272</v>
+      </c>
+      <c r="C89" t="s">
         <v>273</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
+        <v>18</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
         <v>274</v>
-      </c>
-      <c r="C89" t="s">
-        <v>275</v>
-      </c>
-      <c r="E89" t="s">
-        <v>73</v>
-      </c>
-      <c r="F89" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" t="s">
-        <v>38</v>
       </c>
       <c r="H89" t="s">
         <v>14</v>
@@ -4089,16 +4104,16 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
+        <v>275</v>
+      </c>
+      <c r="B90" t="s">
         <v>276</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>277</v>
       </c>
-      <c r="C90" t="s">
-        <v>278</v>
-      </c>
       <c r="E90" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="F90" t="s">
         <v>12</v>
@@ -4112,22 +4127,22 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B91" t="s">
         <v>279</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>280</v>
       </c>
       <c r="E91" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F91" t="s">
         <v>12</v>
       </c>
       <c r="G91" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="H91" t="s">
         <v>14</v>
@@ -4135,22 +4150,22 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B92" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C92" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E92" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="F92" t="s">
         <v>12</v>
       </c>
       <c r="G92" t="s">
-        <v>281</v>
+        <v>222</v>
       </c>
       <c r="H92" t="s">
         <v>14</v>
@@ -4158,7 +4173,7 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B93" t="s">
         <v>282</v>
@@ -4167,13 +4182,13 @@
         <v>17</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="F93" t="s">
         <v>12</v>
       </c>
       <c r="G93" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="H93" t="s">
         <v>14</v>
@@ -4181,22 +4196,22 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B94" t="s">
         <v>284</v>
       </c>
       <c r="C94" t="s">
-        <v>285</v>
+        <v>17</v>
       </c>
       <c r="E94" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F94" t="s">
         <v>12</v>
       </c>
       <c r="G94" t="s">
-        <v>35</v>
+        <v>274</v>
       </c>
       <c r="H94" t="s">
         <v>14</v>
@@ -4204,22 +4219,22 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B95" t="s">
         <v>286</v>
       </c>
       <c r="C95" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="E95" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="F95" t="s">
         <v>12</v>
       </c>
       <c r="G95" t="s">
-        <v>287</v>
+        <v>35</v>
       </c>
       <c r="H95" t="s">
         <v>14</v>
@@ -4227,22 +4242,22 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
+        <v>278</v>
+      </c>
+      <c r="B96" t="s">
         <v>288</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
+        <v>280</v>
+      </c>
+      <c r="E96" t="s">
+        <v>108</v>
+      </c>
+      <c r="F96" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" t="s">
         <v>289</v>
-      </c>
-      <c r="C96" t="s">
-        <v>290</v>
-      </c>
-      <c r="E96" t="s">
-        <v>11</v>
-      </c>
-      <c r="F96" t="s">
-        <v>12</v>
-      </c>
-      <c r="G96" t="s">
-        <v>38</v>
       </c>
       <c r="H96" t="s">
         <v>14</v>
@@ -4250,22 +4265,22 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B97" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C97" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E97" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F97" t="s">
         <v>12</v>
       </c>
       <c r="G97" t="s">
-        <v>291</v>
+        <v>38</v>
       </c>
       <c r="H97" t="s">
         <v>14</v>
@@ -4273,22 +4288,22 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B98" t="s">
+        <v>291</v>
+      </c>
+      <c r="C98" t="s">
         <v>292</v>
       </c>
-      <c r="C98" t="s">
+      <c r="E98" t="s">
+        <v>44</v>
+      </c>
+      <c r="F98" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" t="s">
         <v>293</v>
-      </c>
-      <c r="E98" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" t="s">
-        <v>12</v>
-      </c>
-      <c r="G98" t="s">
-        <v>38</v>
       </c>
       <c r="H98" t="s">
         <v>14</v>
@@ -4296,22 +4311,22 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B99" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C99" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E99" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
       </c>
       <c r="G99" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="H99" t="s">
         <v>14</v>
@@ -4319,7 +4334,7 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B100" t="s">
         <v>294</v>
@@ -4328,13 +4343,13 @@
         <v>295</v>
       </c>
       <c r="E100" t="s">
-        <v>296</v>
+        <v>44</v>
       </c>
       <c r="F100" t="s">
         <v>12</v>
       </c>
       <c r="G100" t="s">
-        <v>196</v>
+        <v>13</v>
       </c>
       <c r="H100" t="s">
         <v>14</v>
@@ -4342,22 +4357,22 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
+        <v>290</v>
+      </c>
+      <c r="B101" t="s">
+        <v>296</v>
+      </c>
+      <c r="C101" t="s">
         <v>297</v>
       </c>
-      <c r="B101" t="s">
+      <c r="E101" t="s">
         <v>298</v>
       </c>
-      <c r="C101" t="s">
-        <v>299</v>
-      </c>
-      <c r="E101" t="s">
-        <v>27</v>
-      </c>
       <c r="F101" t="s">
         <v>12</v>
       </c>
       <c r="G101" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
       <c r="H101" t="s">
         <v>14</v>
@@ -4365,7 +4380,7 @@
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B102" t="s">
         <v>300</v>
@@ -4388,13 +4403,13 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
+        <v>299</v>
+      </c>
+      <c r="B103" t="s">
         <v>302</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>303</v>
-      </c>
-      <c r="C103" t="s">
-        <v>285</v>
       </c>
       <c r="E103" t="s">
         <v>27</v>
@@ -4403,7 +4418,7 @@
         <v>12</v>
       </c>
       <c r="G103" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="H103" t="s">
         <v>14</v>
@@ -4417,16 +4432,16 @@
         <v>305</v>
       </c>
       <c r="C104" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="E104" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F104" t="s">
         <v>12</v>
       </c>
       <c r="G104" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="H104" t="s">
         <v>14</v>
@@ -4434,22 +4449,22 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B105" t="s">
         <v>307</v>
       </c>
       <c r="C105" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E105" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="F105" t="s">
         <v>12</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="H105" t="s">
         <v>14</v>
@@ -4457,16 +4472,16 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B106" t="s">
+        <v>309</v>
+      </c>
+      <c r="C106" t="s">
         <v>308</v>
       </c>
-      <c r="C106" t="s">
-        <v>306</v>
-      </c>
       <c r="E106" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="F106" t="s">
         <v>12</v>
@@ -4480,16 +4495,16 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B107" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C107" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E107" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F107" t="s">
         <v>12</v>
@@ -4503,22 +4518,22 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B108" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C108" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E108" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F108" t="s">
         <v>12</v>
       </c>
       <c r="G108" t="s">
-        <v>196</v>
+        <v>33</v>
       </c>
       <c r="H108" t="s">
         <v>14</v>
@@ -4526,22 +4541,22 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B109" t="s">
         <v>312</v>
       </c>
       <c r="C109" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E109" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="F109" t="s">
         <v>12</v>
       </c>
       <c r="G109" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="H109" t="s">
         <v>14</v>
@@ -4549,16 +4564,16 @@
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B110" t="s">
         <v>314</v>
       </c>
       <c r="C110" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E110" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F110" t="s">
         <v>12</v>
@@ -4572,22 +4587,22 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B111" t="s">
+        <v>316</v>
+      </c>
+      <c r="C111" t="s">
         <v>315</v>
       </c>
-      <c r="C111" t="s">
-        <v>313</v>
-      </c>
       <c r="E111" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F111" t="s">
         <v>12</v>
       </c>
       <c r="G111" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="H111" t="s">
         <v>14</v>
@@ -4595,22 +4610,22 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B112" t="s">
         <v>317</v>
       </c>
       <c r="C112" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E112" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="F112" t="s">
         <v>12</v>
       </c>
       <c r="G112" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="H112" t="s">
         <v>14</v>
@@ -4618,22 +4633,22 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
+        <v>318</v>
+      </c>
+      <c r="B113" t="s">
         <v>319</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>320</v>
       </c>
-      <c r="C113" t="s">
-        <v>321</v>
-      </c>
       <c r="E113" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F113" t="s">
         <v>12</v>
       </c>
       <c r="G113" t="s">
-        <v>322</v>
+        <v>156</v>
       </c>
       <c r="H113" t="s">
         <v>14</v>
@@ -4641,22 +4656,22 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
+        <v>321</v>
+      </c>
+      <c r="B114" t="s">
+        <v>322</v>
+      </c>
+      <c r="C114" t="s">
         <v>323</v>
       </c>
-      <c r="B114" t="s">
+      <c r="E114" t="s">
+        <v>27</v>
+      </c>
+      <c r="F114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" t="s">
         <v>324</v>
-      </c>
-      <c r="C114" t="s">
-        <v>325</v>
-      </c>
-      <c r="E114" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" t="s">
-        <v>78</v>
       </c>
       <c r="H114" t="s">
         <v>14</v>
@@ -4664,7 +4679,7 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B115" t="s">
         <v>326</v>
@@ -4673,7 +4688,7 @@
         <v>327</v>
       </c>
       <c r="E115" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="F115" t="s">
         <v>12</v>
@@ -4687,7 +4702,7 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B116" t="s">
         <v>328</v>
@@ -4696,13 +4711,13 @@
         <v>329</v>
       </c>
       <c r="E116" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="F116" t="s">
         <v>12</v>
       </c>
       <c r="G116" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="H116" t="s">
         <v>14</v>
@@ -4710,7 +4725,7 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B117" t="s">
         <v>330</v>
@@ -4719,13 +4734,13 @@
         <v>331</v>
       </c>
       <c r="E117" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="F117" t="s">
         <v>12</v>
       </c>
       <c r="G117" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="H117" t="s">
         <v>14</v>
@@ -4733,7 +4748,7 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B118" t="s">
         <v>332</v>
@@ -4742,7 +4757,7 @@
         <v>333</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="F118" t="s">
         <v>12</v>
@@ -4756,7 +4771,7 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B119" t="s">
         <v>334</v>
@@ -4779,7 +4794,7 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B120" t="s">
         <v>336</v>
@@ -4788,13 +4803,13 @@
         <v>337</v>
       </c>
       <c r="E120" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F120" t="s">
         <v>12</v>
       </c>
       <c r="G120" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H120" t="s">
         <v>14</v>
@@ -4802,7 +4817,7 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B121" t="s">
         <v>338</v>
@@ -4811,13 +4826,13 @@
         <v>339</v>
       </c>
       <c r="E121" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="F121" t="s">
         <v>12</v>
       </c>
       <c r="G121" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="H121" t="s">
         <v>14</v>
@@ -4825,7 +4840,7 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B122" t="s">
         <v>340</v>
@@ -4848,7 +4863,7 @@
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B123" t="s">
         <v>342</v>
@@ -4856,11 +4871,8 @@
       <c r="C123" t="s">
         <v>343</v>
       </c>
-      <c r="D123" t="s">
-        <v>344</v>
-      </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="F123" t="s">
         <v>12</v>
@@ -4874,12 +4886,15 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B124" t="s">
+        <v>344</v>
+      </c>
+      <c r="C124" t="s">
         <v>345</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>346</v>
       </c>
       <c r="E124" t="s">
@@ -4889,7 +4904,7 @@
         <v>12</v>
       </c>
       <c r="G124" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="H124" t="s">
         <v>14</v>
@@ -4897,25 +4912,22 @@
     </row>
     <row r="125" spans="1:8">
       <c r="A125" t="s">
+        <v>325</v>
+      </c>
+      <c r="B125" t="s">
         <v>347</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>348</v>
       </c>
-      <c r="C125" t="s">
-        <v>349</v>
-      </c>
-      <c r="D125" t="s">
-        <v>350</v>
-      </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F125" t="s">
         <v>12</v>
       </c>
       <c r="G125" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="H125" t="s">
         <v>14</v>
@@ -4923,16 +4935,19 @@
     </row>
     <row r="126" spans="1:8">
       <c r="A126" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B126" t="s">
+        <v>350</v>
+      </c>
+      <c r="C126" t="s">
         <v>351</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>352</v>
       </c>
       <c r="E126" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F126" t="s">
         <v>12</v>
@@ -4946,22 +4961,22 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B127" t="s">
+        <v>350</v>
+      </c>
+      <c r="C127" t="s">
+        <v>351</v>
+      </c>
+      <c r="E127" t="s">
+        <v>34</v>
+      </c>
+      <c r="F127" t="s">
+        <v>12</v>
+      </c>
+      <c r="G127" t="s">
         <v>353</v>
-      </c>
-      <c r="C127" t="s">
-        <v>354</v>
-      </c>
-      <c r="E127" t="s">
-        <v>11</v>
-      </c>
-      <c r="F127" t="s">
-        <v>12</v>
-      </c>
-      <c r="G127" t="s">
-        <v>105</v>
       </c>
       <c r="H127" t="s">
         <v>14</v>
@@ -4969,22 +4984,22 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B128" t="s">
+        <v>354</v>
+      </c>
+      <c r="C128" t="s">
         <v>355</v>
       </c>
-      <c r="C128" t="s">
-        <v>356</v>
-      </c>
       <c r="E128" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F128" t="s">
         <v>12</v>
       </c>
       <c r="G128" t="s">
-        <v>196</v>
+        <v>105</v>
       </c>
       <c r="H128" t="s">
         <v>14</v>
@@ -4992,22 +5007,22 @@
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B129" t="s">
+        <v>356</v>
+      </c>
+      <c r="C129" t="s">
         <v>357</v>
       </c>
-      <c r="C129" t="s">
-        <v>329</v>
-      </c>
       <c r="E129" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="F129" t="s">
         <v>12</v>
       </c>
       <c r="G129" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="H129" t="s">
         <v>14</v>
@@ -5015,7 +5030,7 @@
     </row>
     <row r="130" spans="1:8">
       <c r="A130" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B130" t="s">
         <v>358</v>
@@ -5024,13 +5039,13 @@
         <v>359</v>
       </c>
       <c r="E130" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F130" t="s">
         <v>12</v>
       </c>
       <c r="G130" t="s">
-        <v>71</v>
+        <v>198</v>
       </c>
       <c r="H130" t="s">
         <v>14</v>
@@ -5038,22 +5053,22 @@
     </row>
     <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B131" t="s">
         <v>360</v>
       </c>
       <c r="C131" t="s">
-        <v>254</v>
+        <v>331</v>
       </c>
       <c r="E131" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="F131" t="s">
         <v>12</v>
       </c>
       <c r="G131" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="H131" t="s">
         <v>14</v>
@@ -5061,22 +5076,22 @@
     </row>
     <row r="132" spans="1:8">
       <c r="A132" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B132" t="s">
         <v>361</v>
       </c>
       <c r="C132" t="s">
-        <v>58</v>
+        <v>362</v>
       </c>
       <c r="E132" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F132" t="s">
         <v>12</v>
       </c>
       <c r="G132" t="s">
-        <v>272</v>
+        <v>71</v>
       </c>
       <c r="H132" t="s">
         <v>14</v>
@@ -5084,22 +5099,22 @@
     </row>
     <row r="133" spans="1:8">
       <c r="A133" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="B133" t="s">
         <v>363</v>
       </c>
       <c r="C133" t="s">
-        <v>164</v>
+        <v>256</v>
       </c>
       <c r="E133" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="F133" t="s">
         <v>12</v>
       </c>
       <c r="G133" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H133" t="s">
         <v>14</v>
@@ -5107,22 +5122,22 @@
     </row>
     <row r="134" spans="1:8">
       <c r="A134" t="s">
+        <v>349</v>
+      </c>
+      <c r="B134" t="s">
         <v>364</v>
       </c>
-      <c r="B134" t="s">
-        <v>365</v>
-      </c>
       <c r="C134" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E134" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F134" t="s">
         <v>12</v>
       </c>
       <c r="G134" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="H134" t="s">
         <v>14</v>
@@ -5130,22 +5145,22 @@
     </row>
     <row r="135" spans="1:8">
       <c r="A135" t="s">
+        <v>365</v>
+      </c>
+      <c r="B135" t="s">
         <v>366</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>367</v>
       </c>
-      <c r="C135" t="s">
-        <v>368</v>
-      </c>
       <c r="E135" t="s">
-        <v>369</v>
+        <v>108</v>
       </c>
       <c r="F135" t="s">
         <v>12</v>
       </c>
       <c r="G135" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="H135" t="s">
         <v>14</v>
@@ -5153,22 +5168,22 @@
     </row>
     <row r="136" spans="1:8">
       <c r="A136" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B136" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C136" t="s">
         <v>164</v>
       </c>
       <c r="E136" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F136" t="s">
         <v>12</v>
       </c>
       <c r="G136" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="H136" t="s">
         <v>14</v>
@@ -5176,13 +5191,13 @@
     </row>
     <row r="137" spans="1:8">
       <c r="A137" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B137" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C137" t="s">
-        <v>374</v>
+        <v>14</v>
       </c>
       <c r="E137" t="s">
         <v>18</v>
@@ -5191,7 +5206,7 @@
         <v>12</v>
       </c>
       <c r="G137" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="H137" t="s">
         <v>14</v>
@@ -5199,22 +5214,22 @@
     </row>
     <row r="138" spans="1:8">
       <c r="A138" t="s">
+        <v>372</v>
+      </c>
+      <c r="B138" t="s">
+        <v>373</v>
+      </c>
+      <c r="C138" t="s">
+        <v>374</v>
+      </c>
+      <c r="E138" t="s">
         <v>375</v>
       </c>
-      <c r="B138" t="s">
-        <v>376</v>
-      </c>
-      <c r="C138" t="s">
-        <v>377</v>
-      </c>
-      <c r="E138" t="s">
-        <v>11</v>
-      </c>
       <c r="F138" t="s">
         <v>12</v>
       </c>
       <c r="G138" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="H138" t="s">
         <v>14</v>
@@ -5222,22 +5237,22 @@
     </row>
     <row r="139" spans="1:8">
       <c r="A139" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B139" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C139" t="s">
-        <v>377</v>
+        <v>164</v>
       </c>
       <c r="E139" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F139" t="s">
         <v>12</v>
       </c>
       <c r="G139" t="s">
-        <v>287</v>
+        <v>78</v>
       </c>
       <c r="H139" t="s">
         <v>14</v>
@@ -5245,22 +5260,22 @@
     </row>
     <row r="140" spans="1:8">
       <c r="A140" t="s">
+        <v>378</v>
+      </c>
+      <c r="B140" t="s">
         <v>379</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>380</v>
       </c>
-      <c r="C140" t="s">
-        <v>14</v>
-      </c>
       <c r="E140" t="s">
-        <v>381</v>
+        <v>18</v>
       </c>
       <c r="F140" t="s">
         <v>12</v>
       </c>
       <c r="G140" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H140" t="s">
         <v>14</v>
@@ -5268,22 +5283,22 @@
     </row>
     <row r="141" spans="1:8">
       <c r="A141" t="s">
+        <v>381</v>
+      </c>
+      <c r="B141" t="s">
         <v>382</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>383</v>
       </c>
-      <c r="C141" t="s">
-        <v>384</v>
-      </c>
       <c r="E141" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="F141" t="s">
         <v>12</v>
       </c>
       <c r="G141" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="H141" t="s">
         <v>14</v>
@@ -5291,22 +5306,22 @@
     </row>
     <row r="142" spans="1:8">
       <c r="A142" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B142" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C142" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E142" t="s">
-        <v>388</v>
+        <v>108</v>
       </c>
       <c r="F142" t="s">
         <v>12</v>
       </c>
       <c r="G142" t="s">
-        <v>78</v>
+        <v>289</v>
       </c>
       <c r="H142" t="s">
         <v>14</v>
@@ -5317,19 +5332,19 @@
         <v>385</v>
       </c>
       <c r="B143" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C143" t="s">
-        <v>390</v>
+        <v>14</v>
       </c>
       <c r="E143" t="s">
-        <v>73</v>
+        <v>387</v>
       </c>
       <c r="F143" t="s">
         <v>12</v>
       </c>
       <c r="G143" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="H143" t="s">
         <v>14</v>
@@ -5337,13 +5352,13 @@
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B144" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C144" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E144" t="s">
         <v>133</v>
@@ -5352,7 +5367,7 @@
         <v>12</v>
       </c>
       <c r="G144" t="s">
-        <v>35</v>
+        <v>153</v>
       </c>
       <c r="H144" t="s">
         <v>14</v>
@@ -5360,22 +5375,22 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145" t="s">
+        <v>391</v>
+      </c>
+      <c r="B145" t="s">
         <v>392</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
         <v>393</v>
       </c>
-      <c r="C145" t="s">
+      <c r="E145" t="s">
         <v>394</v>
       </c>
-      <c r="E145" t="s">
-        <v>395</v>
-      </c>
       <c r="F145" t="s">
         <v>12</v>
       </c>
       <c r="G145" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="H145" t="s">
         <v>14</v>
@@ -5383,22 +5398,22 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146" t="s">
+        <v>391</v>
+      </c>
+      <c r="B146" t="s">
+        <v>395</v>
+      </c>
+      <c r="C146" t="s">
         <v>396</v>
       </c>
-      <c r="B146" t="s">
-        <v>397</v>
-      </c>
-      <c r="C146" t="s">
-        <v>398</v>
-      </c>
       <c r="E146" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="F146" t="s">
         <v>12</v>
       </c>
       <c r="G146" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="H146" t="s">
         <v>14</v>
@@ -5406,22 +5421,22 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B147" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C147" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E147" t="s">
-        <v>402</v>
+        <v>133</v>
       </c>
       <c r="F147" t="s">
         <v>12</v>
       </c>
       <c r="G147" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="H147" t="s">
         <v>14</v>
@@ -5429,22 +5444,22 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B148" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C148" t="s">
-        <v>58</v>
+        <v>400</v>
       </c>
       <c r="E148" t="s">
-        <v>11</v>
+        <v>401</v>
       </c>
       <c r="F148" t="s">
         <v>12</v>
       </c>
       <c r="G148" t="s">
-        <v>180</v>
+        <v>38</v>
       </c>
       <c r="H148" t="s">
         <v>14</v>
@@ -5452,22 +5467,22 @@
     </row>
     <row r="149" spans="1:8">
       <c r="A149" t="s">
+        <v>402</v>
+      </c>
+      <c r="B149" t="s">
         <v>403</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>404</v>
       </c>
-      <c r="C149" t="s">
-        <v>14</v>
-      </c>
       <c r="E149" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="F149" t="s">
         <v>12</v>
       </c>
       <c r="G149" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="H149" t="s">
         <v>14</v>
@@ -5475,22 +5490,22 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B150" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C150" t="s">
-        <v>14</v>
+        <v>407</v>
       </c>
       <c r="E150" t="s">
-        <v>11</v>
+        <v>408</v>
       </c>
       <c r="F150" t="s">
         <v>12</v>
       </c>
       <c r="G150" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="H150" t="s">
         <v>14</v>
@@ -5498,22 +5513,22 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B151" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C151" t="s">
         <v>58</v>
       </c>
       <c r="E151" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F151" t="s">
         <v>12</v>
       </c>
       <c r="G151" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="H151" t="s">
         <v>14</v>
@@ -5521,13 +5536,13 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B152" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C152" t="s">
-        <v>410</v>
+        <v>14</v>
       </c>
       <c r="E152" t="s">
         <v>11</v>
@@ -5536,7 +5551,7 @@
         <v>12</v>
       </c>
       <c r="G152" t="s">
-        <v>411</v>
+        <v>128</v>
       </c>
       <c r="H152" t="s">
         <v>14</v>
@@ -5544,13 +5559,13 @@
     </row>
     <row r="153" spans="1:8">
       <c r="A153" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B153" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C153" t="s">
-        <v>414</v>
+        <v>14</v>
       </c>
       <c r="E153" t="s">
         <v>11</v>
@@ -5559,7 +5574,7 @@
         <v>12</v>
       </c>
       <c r="G153" t="s">
-        <v>33</v>
+        <v>156</v>
       </c>
       <c r="H153" t="s">
         <v>14</v>
@@ -5567,13 +5582,13 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B154" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C154" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E154" t="s">
         <v>18</v>
@@ -5582,7 +5597,7 @@
         <v>12</v>
       </c>
       <c r="G154" t="s">
-        <v>417</v>
+        <v>156</v>
       </c>
       <c r="H154" t="s">
         <v>14</v>
@@ -5590,22 +5605,22 @@
     </row>
     <row r="155" spans="1:8">
       <c r="A155" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B155" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C155" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E155" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="F155" t="s">
         <v>12</v>
       </c>
       <c r="G155" t="s">
-        <v>105</v>
+        <v>417</v>
       </c>
       <c r="H155" t="s">
         <v>14</v>
@@ -5613,22 +5628,22 @@
     </row>
     <row r="156" spans="1:8">
       <c r="A156" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B156" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C156" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E156" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F156" t="s">
         <v>12</v>
       </c>
       <c r="G156" t="s">
-        <v>423</v>
+        <v>33</v>
       </c>
       <c r="H156" t="s">
         <v>14</v>
@@ -5636,22 +5651,22 @@
     </row>
     <row r="157" spans="1:8">
       <c r="A157" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B157" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C157" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="E157" t="s">
-        <v>427</v>
+        <v>44</v>
       </c>
       <c r="F157" t="s">
         <v>12</v>
       </c>
       <c r="G157" t="s">
-        <v>428</v>
+        <v>353</v>
       </c>
       <c r="H157" t="s">
         <v>14</v>
@@ -5659,22 +5674,22 @@
     </row>
     <row r="158" spans="1:8">
       <c r="A158" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="B158" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C158" t="s">
-        <v>431</v>
+        <v>77</v>
       </c>
       <c r="E158" t="s">
-        <v>432</v>
+        <v>18</v>
       </c>
       <c r="F158" t="s">
         <v>12</v>
       </c>
       <c r="G158" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="H158" t="s">
         <v>14</v>
@@ -5682,16 +5697,16 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="B159" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C159" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="E159" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="F159" t="s">
         <v>12</v>
@@ -5705,13 +5720,13 @@
     </row>
     <row r="160" spans="1:8">
       <c r="A160" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B160" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="C160" t="s">
-        <v>14</v>
+        <v>428</v>
       </c>
       <c r="E160" t="s">
         <v>27</v>
@@ -5720,7 +5735,7 @@
         <v>12</v>
       </c>
       <c r="G160" t="s">
-        <v>105</v>
+        <v>429</v>
       </c>
       <c r="H160" t="s">
         <v>14</v>
@@ -5728,22 +5743,22 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B161" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C161" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="E161" t="s">
-        <v>27</v>
+        <v>433</v>
       </c>
       <c r="F161" t="s">
         <v>12</v>
       </c>
       <c r="G161" t="s">
-        <v>105</v>
+        <v>434</v>
       </c>
       <c r="H161" t="s">
         <v>14</v>
@@ -5751,22 +5766,22 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162" t="s">
+        <v>435</v>
+      </c>
+      <c r="B162" t="s">
+        <v>436</v>
+      </c>
+      <c r="C162" t="s">
+        <v>437</v>
+      </c>
+      <c r="E162" t="s">
         <v>438</v>
       </c>
-      <c r="B162" t="s">
-        <v>441</v>
-      </c>
-      <c r="C162" t="s">
-        <v>442</v>
-      </c>
-      <c r="E162" t="s">
-        <v>108</v>
-      </c>
       <c r="F162" t="s">
         <v>12</v>
       </c>
       <c r="G162" t="s">
-        <v>105</v>
+        <v>439</v>
       </c>
       <c r="H162" t="s">
         <v>14</v>
@@ -5774,13 +5789,13 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B163" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C163" t="s">
-        <v>444</v>
+        <v>367</v>
       </c>
       <c r="E163" t="s">
         <v>11</v>
@@ -5789,7 +5804,7 @@
         <v>12</v>
       </c>
       <c r="G163" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="H163" t="s">
         <v>14</v>
@@ -5797,22 +5812,22 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B164" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C164" t="s">
-        <v>446</v>
+        <v>14</v>
       </c>
       <c r="E164" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F164" t="s">
         <v>12</v>
       </c>
       <c r="G164" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="H164" t="s">
         <v>14</v>
@@ -5820,25 +5835,22 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B165" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C165" t="s">
-        <v>449</v>
-      </c>
-      <c r="D165" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E165" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F165" t="s">
         <v>12</v>
       </c>
       <c r="G165" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="H165" t="s">
         <v>14</v>
@@ -5846,22 +5858,22 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B166" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="C166" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E166" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="F166" t="s">
         <v>12</v>
       </c>
       <c r="G166" t="s">
-        <v>454</v>
+        <v>105</v>
       </c>
       <c r="H166" t="s">
         <v>14</v>
@@ -5869,22 +5881,22 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B167" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C167" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E167" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F167" t="s">
         <v>12</v>
       </c>
       <c r="G167" t="s">
-        <v>454</v>
+        <v>137</v>
       </c>
       <c r="H167" t="s">
         <v>14</v>
@@ -5892,22 +5904,22 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="B168" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="C168" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="E168" t="s">
-        <v>460</v>
+        <v>18</v>
       </c>
       <c r="F168" t="s">
         <v>12</v>
       </c>
       <c r="G168" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="H168" t="s">
         <v>14</v>
@@ -5915,22 +5927,25 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B169" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C169" t="s">
-        <v>463</v>
+        <v>454</v>
+      </c>
+      <c r="D169" t="s">
+        <v>455</v>
       </c>
       <c r="E169" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="F169" t="s">
         <v>12</v>
       </c>
       <c r="G169" t="s">
-        <v>423</v>
+        <v>83</v>
       </c>
       <c r="H169" t="s">
         <v>14</v>
@@ -5938,25 +5953,22 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B170" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C170" t="s">
-        <v>465</v>
-      </c>
-      <c r="D170" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="E170" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="F170" t="s">
         <v>12</v>
       </c>
       <c r="G170" t="s">
-        <v>423</v>
+        <v>459</v>
       </c>
       <c r="H170" t="s">
         <v>14</v>
@@ -5964,25 +5976,22 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171" t="s">
+        <v>456</v>
+      </c>
+      <c r="B171" t="s">
+        <v>460</v>
+      </c>
+      <c r="C171" t="s">
         <v>461</v>
       </c>
-      <c r="B171" t="s">
-        <v>467</v>
-      </c>
-      <c r="C171" t="s">
-        <v>468</v>
-      </c>
-      <c r="D171" t="s">
-        <v>469</v>
-      </c>
       <c r="E171" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="F171" t="s">
         <v>12</v>
       </c>
       <c r="G171" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="H171" t="s">
         <v>14</v>
@@ -5990,22 +5999,22 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B172" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C172" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E172" t="s">
-        <v>86</v>
+        <v>465</v>
       </c>
       <c r="F172" t="s">
         <v>12</v>
       </c>
       <c r="G172" t="s">
-        <v>470</v>
+        <v>153</v>
       </c>
       <c r="H172" t="s">
         <v>14</v>
@@ -6013,10 +6022,10 @@
     </row>
     <row r="173" spans="1:8">
       <c r="A173" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B173" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C173" t="s">
         <v>468</v>
@@ -6028,7 +6037,7 @@
         <v>12</v>
       </c>
       <c r="G173" t="s">
-        <v>153</v>
+        <v>429</v>
       </c>
       <c r="H173" t="s">
         <v>14</v>
@@ -6036,22 +6045,25 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B174" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C174" t="s">
-        <v>475</v>
+        <v>470</v>
+      </c>
+      <c r="D174" t="s">
+        <v>471</v>
       </c>
       <c r="E174" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="F174" t="s">
         <v>12</v>
       </c>
       <c r="G174" t="s">
-        <v>153</v>
+        <v>429</v>
       </c>
       <c r="H174" t="s">
         <v>14</v>
@@ -6059,22 +6071,25 @@
     </row>
     <row r="175" spans="1:8">
       <c r="A175" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B175" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C175" t="s">
-        <v>14</v>
+        <v>473</v>
+      </c>
+      <c r="D175" t="s">
+        <v>474</v>
       </c>
       <c r="E175" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="F175" t="s">
         <v>12</v>
       </c>
       <c r="G175" t="s">
-        <v>19</v>
+        <v>475</v>
       </c>
       <c r="H175" t="s">
         <v>14</v>
@@ -6082,22 +6097,22 @@
     </row>
     <row r="176" spans="1:8">
       <c r="A176" t="s">
+        <v>466</v>
+      </c>
+      <c r="B176" t="s">
         <v>476</v>
       </c>
-      <c r="B176" t="s">
-        <v>478</v>
-      </c>
       <c r="C176" t="s">
-        <v>14</v>
+        <v>473</v>
       </c>
       <c r="E176" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="F176" t="s">
         <v>12</v>
       </c>
       <c r="G176" t="s">
-        <v>213</v>
+        <v>475</v>
       </c>
       <c r="H176" t="s">
         <v>14</v>
@@ -6105,22 +6120,22 @@
     </row>
     <row r="177" spans="1:8">
       <c r="A177" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B177" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C177" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="E177" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="F177" t="s">
         <v>12</v>
       </c>
       <c r="G177" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="H177" t="s">
         <v>14</v>
@@ -6128,22 +6143,22 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B178" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C178" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="E178" t="s">
-        <v>485</v>
+        <v>114</v>
       </c>
       <c r="F178" t="s">
         <v>12</v>
       </c>
       <c r="G178" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
       <c r="H178" t="s">
         <v>14</v>
@@ -6151,22 +6166,22 @@
     </row>
     <row r="179" spans="1:8">
       <c r="A179" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B179" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C179" t="s">
-        <v>488</v>
+        <v>14</v>
       </c>
       <c r="E179" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F179" t="s">
         <v>12</v>
       </c>
       <c r="G179" t="s">
-        <v>217</v>
+        <v>19</v>
       </c>
       <c r="H179" t="s">
         <v>14</v>
@@ -6174,22 +6189,22 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B180" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="C180" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E180" t="s">
-        <v>402</v>
+        <v>27</v>
       </c>
       <c r="F180" t="s">
         <v>12</v>
       </c>
       <c r="G180" t="s">
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="H180" t="s">
         <v>14</v>
@@ -6197,13 +6212,13 @@
     </row>
     <row r="181" spans="1:8">
       <c r="A181" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B181" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="C181" t="s">
-        <v>14</v>
+        <v>486</v>
       </c>
       <c r="E181" t="s">
         <v>11</v>
@@ -6212,7 +6227,7 @@
         <v>12</v>
       </c>
       <c r="G181" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
       <c r="H181" t="s">
         <v>14</v>
@@ -6220,22 +6235,22 @@
     </row>
     <row r="182" spans="1:8">
       <c r="A182" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B182" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="C182" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="E182" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="F182" t="s">
         <v>12</v>
       </c>
       <c r="G182" t="s">
-        <v>137</v>
+        <v>222</v>
       </c>
       <c r="H182" t="s">
         <v>14</v>
@@ -6243,22 +6258,22 @@
     </row>
     <row r="183" spans="1:8">
       <c r="A183" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B183" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C183" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="E183" t="s">
-        <v>460</v>
+        <v>44</v>
       </c>
       <c r="F183" t="s">
         <v>12</v>
       </c>
       <c r="G183" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
       <c r="H183" t="s">
         <v>14</v>
@@ -6266,22 +6281,22 @@
     </row>
     <row r="184" spans="1:8">
       <c r="A184" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B184" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C184" t="s">
-        <v>501</v>
+        <v>17</v>
       </c>
       <c r="E184" t="s">
-        <v>18</v>
+        <v>408</v>
       </c>
       <c r="F184" t="s">
         <v>12</v>
       </c>
       <c r="G184" t="s">
-        <v>244</v>
+        <v>153</v>
       </c>
       <c r="H184" t="s">
         <v>14</v>
@@ -6289,13 +6304,13 @@
     </row>
     <row r="185" spans="1:8">
       <c r="A185" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="B185" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C185" t="s">
-        <v>504</v>
+        <v>14</v>
       </c>
       <c r="E185" t="s">
         <v>11</v>
@@ -6304,7 +6319,7 @@
         <v>12</v>
       </c>
       <c r="G185" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="H185" t="s">
         <v>14</v>
@@ -6312,22 +6327,22 @@
     </row>
     <row r="186" spans="1:8">
       <c r="A186" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B186" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C186" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="E186" t="s">
-        <v>27</v>
+        <v>490</v>
       </c>
       <c r="F186" t="s">
         <v>12</v>
       </c>
       <c r="G186" t="s">
-        <v>252</v>
+        <v>137</v>
       </c>
       <c r="H186" t="s">
         <v>14</v>
@@ -6335,22 +6350,22 @@
     </row>
     <row r="187" spans="1:8">
       <c r="A187" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B187" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="C187" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="E187" t="s">
-        <v>18</v>
+        <v>465</v>
       </c>
       <c r="F187" t="s">
         <v>12</v>
       </c>
       <c r="G187" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="H187" t="s">
         <v>14</v>
@@ -6358,22 +6373,22 @@
     </row>
     <row r="188" spans="1:8">
       <c r="A188" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B188" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="C188" t="s">
-        <v>58</v>
+        <v>506</v>
       </c>
       <c r="E188" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F188" t="s">
         <v>12</v>
       </c>
       <c r="G188" t="s">
-        <v>19</v>
+        <v>246</v>
       </c>
       <c r="H188" t="s">
         <v>14</v>
@@ -6381,22 +6396,22 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="B189" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C189" t="s">
-        <v>17</v>
+        <v>509</v>
       </c>
       <c r="E189" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="F189" t="s">
         <v>12</v>
       </c>
       <c r="G189" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H189" t="s">
         <v>14</v>
@@ -6404,22 +6419,22 @@
     </row>
     <row r="190" spans="1:8">
       <c r="A190" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B190" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="C190" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="E190" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="F190" t="s">
         <v>12</v>
       </c>
       <c r="G190" t="s">
-        <v>63</v>
+        <v>254</v>
       </c>
       <c r="H190" t="s">
         <v>14</v>
@@ -6427,22 +6442,22 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B191" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="C191" t="s">
-        <v>14</v>
+        <v>515</v>
       </c>
       <c r="E191" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="F191" t="s">
         <v>12</v>
       </c>
       <c r="G191" t="s">
-        <v>520</v>
+        <v>83</v>
       </c>
       <c r="H191" t="s">
         <v>14</v>
@@ -6450,22 +6465,22 @@
     </row>
     <row r="192" spans="1:8">
       <c r="A192" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B192" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C192" t="s">
-        <v>523</v>
+        <v>58</v>
       </c>
       <c r="E192" t="s">
-        <v>240</v>
+        <v>27</v>
       </c>
       <c r="F192" t="s">
         <v>12</v>
       </c>
       <c r="G192" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="H192" t="s">
         <v>14</v>
@@ -6473,22 +6488,22 @@
     </row>
     <row r="193" spans="1:8">
       <c r="A193" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="B193" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C193" t="s">
-        <v>526</v>
+        <v>17</v>
       </c>
       <c r="E193" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="F193" t="s">
         <v>12</v>
       </c>
       <c r="G193" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="H193" t="s">
         <v>14</v>
@@ -6496,22 +6511,22 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B194" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C194" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E194" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F194" t="s">
         <v>12</v>
       </c>
       <c r="G194" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
       <c r="H194" t="s">
         <v>14</v>
@@ -6519,25 +6534,22 @@
     </row>
     <row r="195" spans="1:8">
       <c r="A195" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="B195" t="s">
-        <v>96</v>
+        <v>524</v>
       </c>
       <c r="C195" t="s">
-        <v>349</v>
-      </c>
-      <c r="D195" t="s">
-        <v>186</v>
+        <v>14</v>
       </c>
       <c r="E195" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="F195" t="s">
         <v>12</v>
       </c>
       <c r="G195" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="H195" t="s">
         <v>14</v>
@@ -6545,25 +6557,22 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" t="s">
+        <v>526</v>
+      </c>
+      <c r="B196" t="s">
+        <v>527</v>
+      </c>
+      <c r="C196" t="s">
         <v>528</v>
       </c>
-      <c r="B196" t="s">
-        <v>530</v>
-      </c>
-      <c r="C196" t="s">
-        <v>58</v>
-      </c>
-      <c r="D196" t="s">
-        <v>531</v>
-      </c>
       <c r="E196" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="F196" t="s">
         <v>12</v>
       </c>
       <c r="G196" t="s">
-        <v>529</v>
+        <v>71</v>
       </c>
       <c r="H196" t="s">
         <v>14</v>
@@ -6571,25 +6580,22 @@
     </row>
     <row r="197" spans="1:8">
       <c r="A197" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B197" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C197" t="s">
-        <v>327</v>
-      </c>
-      <c r="D197" t="s">
-        <v>349</v>
+        <v>531</v>
       </c>
       <c r="E197" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F197" t="s">
         <v>12</v>
       </c>
       <c r="G197" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="H197" t="s">
         <v>14</v>
@@ -6597,16 +6603,13 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B198" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C198" t="s">
-        <v>327</v>
-      </c>
-      <c r="D198" t="s">
-        <v>349</v>
+        <v>531</v>
       </c>
       <c r="E198" t="s">
         <v>108</v>
@@ -6615,7 +6618,7 @@
         <v>12</v>
       </c>
       <c r="G198" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="H198" t="s">
         <v>14</v>
@@ -6623,13 +6626,16 @@
     </row>
     <row r="199" spans="1:8">
       <c r="A199" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B199" t="s">
-        <v>535</v>
+        <v>96</v>
       </c>
       <c r="C199" t="s">
-        <v>536</v>
+        <v>351</v>
+      </c>
+      <c r="D199" t="s">
+        <v>188</v>
       </c>
       <c r="E199" t="s">
         <v>18</v>
@@ -6638,7 +6644,7 @@
         <v>12</v>
       </c>
       <c r="G199" t="s">
-        <v>95</v>
+        <v>534</v>
       </c>
       <c r="H199" t="s">
         <v>14</v>
@@ -6646,22 +6652,25 @@
     </row>
     <row r="200" spans="1:8">
       <c r="A200" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B200" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C200" t="s">
-        <v>14</v>
+        <v>58</v>
+      </c>
+      <c r="D200" t="s">
+        <v>536</v>
       </c>
       <c r="E200" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F200" t="s">
         <v>12</v>
       </c>
       <c r="G200" t="s">
-        <v>55</v>
+        <v>534</v>
       </c>
       <c r="H200" t="s">
         <v>14</v>
@@ -6669,22 +6678,25 @@
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
+        <v>533</v>
+      </c>
+      <c r="B201" t="s">
         <v>537</v>
       </c>
-      <c r="B201" t="s">
-        <v>539</v>
-      </c>
       <c r="C201" t="s">
-        <v>14</v>
+        <v>329</v>
+      </c>
+      <c r="D201" t="s">
+        <v>351</v>
       </c>
       <c r="E201" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="F201" t="s">
         <v>12</v>
       </c>
       <c r="G201" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H201" t="s">
         <v>14</v>
@@ -6692,22 +6704,25 @@
     </row>
     <row r="202" spans="1:8">
       <c r="A202" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B202" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C202" t="s">
-        <v>14</v>
+        <v>329</v>
+      </c>
+      <c r="D202" t="s">
+        <v>351</v>
       </c>
       <c r="E202" t="s">
-        <v>540</v>
+        <v>108</v>
       </c>
       <c r="F202" t="s">
         <v>12</v>
       </c>
       <c r="G202" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="H202" t="s">
         <v>14</v>
@@ -6715,22 +6730,22 @@
     </row>
     <row r="203" spans="1:8">
       <c r="A203" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B203" t="s">
+        <v>540</v>
+      </c>
+      <c r="C203" t="s">
         <v>541</v>
       </c>
-      <c r="C203" t="s">
-        <v>14</v>
-      </c>
       <c r="E203" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="F203" t="s">
         <v>12</v>
       </c>
       <c r="G203" t="s">
-        <v>291</v>
+        <v>95</v>
       </c>
       <c r="H203" t="s">
         <v>14</v>
@@ -6744,7 +6759,7 @@
         <v>543</v>
       </c>
       <c r="C204" t="s">
-        <v>544</v>
+        <v>14</v>
       </c>
       <c r="E204" t="s">
         <v>11</v>
@@ -6753,7 +6768,7 @@
         <v>12</v>
       </c>
       <c r="G204" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="H204" t="s">
         <v>14</v>
@@ -6761,22 +6776,22 @@
     </row>
     <row r="205" spans="1:8">
       <c r="A205" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B205" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C205" t="s">
         <v>14</v>
       </c>
       <c r="E205" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="F205" t="s">
         <v>12</v>
       </c>
       <c r="G205" t="s">
-        <v>520</v>
+        <v>55</v>
       </c>
       <c r="H205" t="s">
         <v>14</v>
@@ -6784,22 +6799,22 @@
     </row>
     <row r="206" spans="1:8">
       <c r="A206" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B206" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C206" t="s">
-        <v>549</v>
+        <v>14</v>
       </c>
       <c r="E206" t="s">
-        <v>18</v>
+        <v>545</v>
       </c>
       <c r="F206" t="s">
         <v>12</v>
       </c>
       <c r="G206" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="H206" t="s">
         <v>14</v>
@@ -6807,24 +6822,116 @@
     </row>
     <row r="207" spans="1:8">
       <c r="A207" t="s">
+        <v>542</v>
+      </c>
+      <c r="B207" t="s">
+        <v>546</v>
+      </c>
+      <c r="C207" t="s">
+        <v>14</v>
+      </c>
+      <c r="E207" t="s">
+        <v>108</v>
+      </c>
+      <c r="F207" t="s">
+        <v>12</v>
+      </c>
+      <c r="G207" t="s">
+        <v>293</v>
+      </c>
+      <c r="H207" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8">
+      <c r="A208" t="s">
+        <v>547</v>
+      </c>
+      <c r="B208" t="s">
+        <v>548</v>
+      </c>
+      <c r="C208" t="s">
+        <v>549</v>
+      </c>
+      <c r="E208" t="s">
+        <v>11</v>
+      </c>
+      <c r="F208" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" t="s">
+        <v>13</v>
+      </c>
+      <c r="H208" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8">
+      <c r="A209" t="s">
         <v>550</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B209" t="s">
         <v>551</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C209" t="s">
+        <v>14</v>
+      </c>
+      <c r="E209" t="s">
+        <v>11</v>
+      </c>
+      <c r="F209" t="s">
+        <v>12</v>
+      </c>
+      <c r="G209" t="s">
+        <v>525</v>
+      </c>
+      <c r="H209" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8">
+      <c r="A210" t="s">
         <v>552</v>
       </c>
-      <c r="E207" t="s">
+      <c r="B210" t="s">
+        <v>553</v>
+      </c>
+      <c r="C210" t="s">
+        <v>554</v>
+      </c>
+      <c r="E210" t="s">
         <v>18</v>
       </c>
-      <c r="F207" t="s">
-        <v>12</v>
-      </c>
-      <c r="G207" t="s">
-        <v>220</v>
-      </c>
-      <c r="H207" t="s">
+      <c r="F210" t="s">
+        <v>12</v>
+      </c>
+      <c r="G210" t="s">
+        <v>98</v>
+      </c>
+      <c r="H210" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8">
+      <c r="A211" t="s">
+        <v>555</v>
+      </c>
+      <c r="B211" t="s">
+        <v>556</v>
+      </c>
+      <c r="C211" t="s">
+        <v>557</v>
+      </c>
+      <c r="E211" t="s">
+        <v>18</v>
+      </c>
+      <c r="F211" t="s">
+        <v>12</v>
+      </c>
+      <c r="G211" t="s">
+        <v>222</v>
+      </c>
+      <c r="H211" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>